<commit_message>
Share Button Changes rani(Done)
</commit_message>
<xml_diff>
--- a/DailyBibleverses.xlsx
+++ b/DailyBibleverses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Agape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6ACA76-CB0B-4312-B97A-5D45135A3978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC256D8-B177-428F-ADB6-A5F86324FDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{81CB52D9-4E9C-4138-8F80-F25C7BA19DB4}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Isaiah 41:10</t>
   </si>
   <si>
-    <t>So do not fear, for I am with you..."</t>
-  </si>
-  <si>
     <t>God's promise of His presence dispels fear and anxiety. We are reminded that we are never alone, which brings comfort and courage during challenging times.</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>This verse encourages spiritual strength and reliance on God's power rather than our own, preparing us for challenges ahead.</t>
+  </si>
+  <si>
+    <t>"So do not fear, for I am with you..."</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,223 +620,223 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1">
         <v>45627</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>45628</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>45629</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="1">
         <v>45630</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>45631</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>45632</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>45633</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1">
         <v>45634</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
       </c>
       <c r="C11" s="1">
         <v>45635</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
       </c>
       <c r="C12" s="1">
         <v>45636</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
       </c>
       <c r="C13" s="1">
         <v>45637</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
       </c>
       <c r="C14" s="1">
         <v>45638</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
       </c>
       <c r="C15" s="1">
         <v>45639</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
       </c>
       <c r="C16" s="1">
         <v>45640</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
         <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
       </c>
       <c r="C17" s="1">
         <v>45641</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
       </c>
       <c r="C18" s="1">
         <v>45642</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>